<commit_message>
add data - 10k plus votes for balen
</commit_message>
<xml_diff>
--- a/margin.xlsx
+++ b/margin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Last_Update</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">5/17/2022 7:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/17/2022 8:30</t>
   </si>
 </sst>
 </file>
@@ -234,13 +237,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.01"/>
   </cols>
@@ -901,6 +904,28 @@
       <c r="F30" s="1" t="n">
         <f aca="false">B30-D30</f>
         <v>5164</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>10359</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>5515</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>4792</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <f aca="false">B31-C31</f>
+        <v>4844</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <f aca="false">B31-D31</f>
+        <v>5567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Congratulations Balen :tada: :tada: :tada:
</commit_message>
<xml_diff>
--- a/margin.xlsx
+++ b/margin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t xml:space="preserve">Last_Update</t>
   </si>
@@ -421,7 +421,16 @@
     <t xml:space="preserve">5/25/2022 6:00</t>
   </si>
   <si>
-    <t xml:space="preserve">5/25/2022 6:47</t>
+    <t xml:space="preserve">5/25/2022 8:48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/25/2022 10:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/25/2022 10:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/25/2022 11:10</t>
   </si>
 </sst>
 </file>
@@ -531,13 +540,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G127" activeCellId="0" sqref="G127"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A117" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G137" activeCellId="0" sqref="G137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.01"/>
   </cols>
@@ -4323,29 +4332,119 @@
         <v>133</v>
       </c>
       <c r="B127" s="3" t="n">
-        <v>54748</v>
+        <v>54870</v>
       </c>
       <c r="C127" s="3" t="n">
-        <v>33990</v>
+        <v>34036</v>
       </c>
       <c r="D127" s="3" t="n">
-        <v>34621</v>
+        <v>34668</v>
       </c>
       <c r="E127" s="1" t="n">
         <f aca="false">B127-C127</f>
-        <v>20758</v>
+        <v>20834</v>
       </c>
       <c r="F127" s="1" t="n">
         <f aca="false">B127-D127</f>
-        <v>20127</v>
+        <v>20202</v>
       </c>
       <c r="G127" s="0" t="n">
         <f aca="false">B127/C127</f>
-        <v>1.61070903206826</v>
+        <v>1.61211658244212</v>
       </c>
       <c r="H127" s="0" t="n">
         <f aca="false">B127/D127</f>
-        <v>1.58135235839519</v>
+        <v>1.58272758740048</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B128" s="3" t="n">
+        <v>55458</v>
+      </c>
+      <c r="C128" s="3" t="n">
+        <v>34459</v>
+      </c>
+      <c r="D128" s="3" t="n">
+        <v>34104</v>
+      </c>
+      <c r="E128" s="1" t="n">
+        <f aca="false">B128-C128</f>
+        <v>20999</v>
+      </c>
+      <c r="F128" s="1" t="n">
+        <f aca="false">B128-D128</f>
+        <v>21354</v>
+      </c>
+      <c r="G128" s="0" t="n">
+        <f aca="false">B128/C128</f>
+        <v>1.60939087030964</v>
+      </c>
+      <c r="H128" s="0" t="n">
+        <f aca="false">B128/D128</f>
+        <v>1.62614356087263</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B129" s="3" t="n">
+        <v>55480</v>
+      </c>
+      <c r="C129" s="3" t="n">
+        <v>34475</v>
+      </c>
+      <c r="D129" s="3" t="n">
+        <v>35119</v>
+      </c>
+      <c r="E129" s="1" t="n">
+        <f aca="false">B129-C129</f>
+        <v>21005</v>
+      </c>
+      <c r="F129" s="1" t="n">
+        <f aca="false">B129-D129</f>
+        <v>20361</v>
+      </c>
+      <c r="G129" s="0" t="n">
+        <f aca="false">B129/C129</f>
+        <v>1.60928208846991</v>
+      </c>
+      <c r="H129" s="0" t="n">
+        <f aca="false">B129/D129</f>
+        <v>1.57977163358866</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B130" s="3" t="n">
+        <v>55747</v>
+      </c>
+      <c r="C130" s="3" t="n">
+        <v>34626</v>
+      </c>
+      <c r="D130" s="3" t="n">
+        <v>35372</v>
+      </c>
+      <c r="E130" s="1" t="n">
+        <f aca="false">B130-C130</f>
+        <v>21121</v>
+      </c>
+      <c r="F130" s="1" t="n">
+        <f aca="false">B130-D130</f>
+        <v>20375</v>
+      </c>
+      <c r="G130" s="0" t="n">
+        <f aca="false">B130/C130</f>
+        <v>1.60997516317218</v>
+      </c>
+      <c r="H130" s="0" t="n">
+        <f aca="false">B130/D130</f>
+        <v>1.57602058125071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Count - Congrats Balen :tada: :tada:
</commit_message>
<xml_diff>
--- a/margin.xlsx
+++ b/margin.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t xml:space="preserve">Last_Update</t>
   </si>
@@ -424,19 +424,34 @@
     <t xml:space="preserve">5/25/2022 8:48</t>
   </si>
   <si>
-    <t xml:space="preserve">5/25/2022 10:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/25/2022 10:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/25/2022 11:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/25/2022 13:25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5/25/2022 14:34</t>
+    <t xml:space="preserve">5/26/2022 10:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/26/2022 10:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/26/2022 11:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/26/2022 13:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/26/2022 14:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/26/2022 16:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/26/2022 18:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/26/2022 21:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/26/2022 9:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5/26/2022 23:00</t>
   </si>
 </sst>
 </file>
@@ -546,13 +561,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H132"/>
+  <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A93" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G127" activeCellId="0" sqref="G127"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A116" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:H137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.01"/>
   </cols>
@@ -4511,6 +4526,156 @@
       <c r="H132" s="0" t="n">
         <f aca="false">B132/D132</f>
         <v>1.58147340157745</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B133" s="3" t="n">
+        <v>56830</v>
+      </c>
+      <c r="C133" s="3" t="n">
+        <v>35311</v>
+      </c>
+      <c r="D133" s="3" t="n">
+        <v>35918</v>
+      </c>
+      <c r="E133" s="1" t="n">
+        <f aca="false">B133-C133</f>
+        <v>21519</v>
+      </c>
+      <c r="F133" s="1" t="n">
+        <f aca="false">B133-D133</f>
+        <v>20912</v>
+      </c>
+      <c r="G133" s="0" t="n">
+        <f aca="false">B133/C133</f>
+        <v>1.6094134972105</v>
+      </c>
+      <c r="H133" s="0" t="n">
+        <f aca="false">B133/D133</f>
+        <v>1.58221504538115</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B134" s="3" t="n">
+        <v>57336</v>
+      </c>
+      <c r="C134" s="3" t="n">
+        <v>35727</v>
+      </c>
+      <c r="D134" s="3" t="n">
+        <v>36266</v>
+      </c>
+      <c r="E134" s="1" t="n">
+        <f aca="false">B134-C134</f>
+        <v>21609</v>
+      </c>
+      <c r="F134" s="1" t="n">
+        <f aca="false">B134-D134</f>
+        <v>21070</v>
+      </c>
+      <c r="G134" s="0" t="n">
+        <f aca="false">B134/C134</f>
+        <v>1.60483667814258</v>
+      </c>
+      <c r="H134" s="0" t="n">
+        <f aca="false">B134/D134</f>
+        <v>1.58098494457619</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B135" s="3" t="n">
+        <v>57387</v>
+      </c>
+      <c r="C135" s="3" t="n">
+        <v>35755</v>
+      </c>
+      <c r="D135" s="3" t="n">
+        <v>36292</v>
+      </c>
+      <c r="E135" s="1" t="n">
+        <f aca="false">B135-C135</f>
+        <v>21632</v>
+      </c>
+      <c r="F135" s="1" t="n">
+        <f aca="false">B135-D135</f>
+        <v>21095</v>
+      </c>
+      <c r="G135" s="0" t="n">
+        <f aca="false">B135/C135</f>
+        <v>1.60500629282618</v>
+      </c>
+      <c r="H135" s="0" t="n">
+        <f aca="false">B135/D135</f>
+        <v>1.58125757742753</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B136" s="3" t="n">
+        <v>59149</v>
+      </c>
+      <c r="C136" s="3" t="n">
+        <v>37218</v>
+      </c>
+      <c r="D136" s="3" t="n">
+        <v>37542</v>
+      </c>
+      <c r="E136" s="1" t="n">
+        <f aca="false">B136-C136</f>
+        <v>21931</v>
+      </c>
+      <c r="F136" s="1" t="n">
+        <f aca="false">B136-D136</f>
+        <v>21607</v>
+      </c>
+      <c r="G136" s="0" t="n">
+        <f aca="false">B136/C136</f>
+        <v>1.58925788596915</v>
+      </c>
+      <c r="H136" s="0" t="n">
+        <f aca="false">B136/D136</f>
+        <v>1.57554205955996</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B137" s="3" t="n">
+        <v>61767</v>
+      </c>
+      <c r="C137" s="3" t="n">
+        <v>38117</v>
+      </c>
+      <c r="D137" s="3" t="n">
+        <v>38341</v>
+      </c>
+      <c r="E137" s="1" t="n">
+        <f aca="false">B137-C137</f>
+        <v>23650</v>
+      </c>
+      <c r="F137" s="1" t="n">
+        <f aca="false">B137-D137</f>
+        <v>23426</v>
+      </c>
+      <c r="G137" s="0" t="n">
+        <f aca="false">B137/C137</f>
+        <v>1.62045806333132</v>
+      </c>
+      <c r="H137" s="0" t="n">
+        <f aca="false">B137/D137</f>
+        <v>1.6109908453092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>